<commit_message>
lots of changes to tweak code and produce new figures for paper
</commit_message>
<xml_diff>
--- a/data/data_extraction.xlsx
+++ b/data/data_extraction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\work\Projects\In_progress\precip_changes_soil_fauna\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766A2851-6644-4C3B-878D-E3175328CAE9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4AE8968-9A73-413F-A34A-0E74DDA74732}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">articles!$A$1:$K$39</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">outcomes!$A$1:$AR$666</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">outcomes!$A$1:$AR$752</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">taxonomy!$A$2:$M$87</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -3798,8 +3798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55AD3176-A41F-4F7C-892D-39B873D09377}">
   <dimension ref="A1:V47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="U46" sqref="U46"/>
     </sheetView>
@@ -7027,11 +7027,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0B0D52E-D3B5-4A8D-9024-54955AA3F695}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AR752"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T752" sqref="T752"/>
+      <selection pane="bottomLeft" activeCell="P753" sqref="P753"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8683,7 +8684,7 @@
         <v>6.3426359000000002E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>286</v>
       </c>
@@ -17236,7 +17237,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="89" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>302</v>
       </c>
@@ -20729,7 +20730,7 @@
         <v>1.0651352540000001</v>
       </c>
     </row>
-    <row r="118" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>322</v>
       </c>
@@ -20845,7 +20846,7 @@
         <v>1.0651352540000001</v>
       </c>
     </row>
-    <row r="119" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>322</v>
       </c>
@@ -21077,7 +21078,7 @@
         <v>1.0651352540000001</v>
       </c>
     </row>
-    <row r="121" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>322</v>
       </c>
@@ -21702,7 +21703,7 @@
         <v>1.115829446</v>
       </c>
     </row>
-    <row r="126" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>322</v>
       </c>
@@ -21818,7 +21819,7 @@
         <v>1.115829446</v>
       </c>
     </row>
-    <row r="127" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>322</v>
       </c>
@@ -22050,7 +22051,7 @@
         <v>1.115829446</v>
       </c>
     </row>
-    <row r="129" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>322</v>
       </c>
@@ -22300,7 +22301,7 @@
         <v>1.0651352540000001</v>
       </c>
     </row>
-    <row r="131" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>322</v>
       </c>
@@ -22416,7 +22417,7 @@
         <v>1.0651352540000001</v>
       </c>
     </row>
-    <row r="132" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>322</v>
       </c>
@@ -22648,7 +22649,7 @@
         <v>1.0651352540000001</v>
       </c>
     </row>
-    <row r="134" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>322</v>
       </c>
@@ -23270,7 +23271,7 @@
         <v>1.115829446</v>
       </c>
     </row>
-    <row r="139" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>322</v>
       </c>
@@ -23386,7 +23387,7 @@
         <v>1.115829446</v>
       </c>
     </row>
-    <row r="140" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>322</v>
       </c>
@@ -23618,7 +23619,7 @@
         <v>1.115829446</v>
       </c>
     </row>
-    <row r="142" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>322</v>
       </c>
@@ -35891,7 +35892,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="244" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>348</v>
       </c>
@@ -35992,7 +35993,7 @@
         <v>1.0651352540000001</v>
       </c>
     </row>
-    <row r="245" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>348</v>
       </c>
@@ -36093,7 +36094,7 @@
         <v>1.0651352540000001</v>
       </c>
     </row>
-    <row r="246" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>348</v>
       </c>
@@ -38726,7 +38727,7 @@
         <v>6.3426359000000002E-2</v>
       </c>
     </row>
-    <row r="271" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>354</v>
       </c>
@@ -39779,7 +39780,7 @@
         <v>1.0651352540000001</v>
       </c>
     </row>
-    <row r="280" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>363</v>
       </c>
@@ -40124,7 +40125,7 @@
         <v>1.115829446</v>
       </c>
     </row>
-    <row r="283" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>363</v>
       </c>
@@ -40689,7 +40690,7 @@
         <v>1.0651352540000001</v>
       </c>
     </row>
-    <row r="288" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>363</v>
       </c>
@@ -41144,7 +41145,7 @@
         <v>1.115829446</v>
       </c>
     </row>
-    <row r="292" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>363</v>
       </c>
@@ -41599,7 +41600,7 @@
         <v>1.0651352540000001</v>
       </c>
     </row>
-    <row r="296" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>363</v>
       </c>
@@ -42054,7 +42055,7 @@
         <v>1.115829446</v>
       </c>
     </row>
-    <row r="300" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>363</v>
       </c>
@@ -43241,7 +43242,7 @@
         <v>1.115829446</v>
       </c>
     </row>
-    <row r="310" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>372</v>
       </c>
@@ -43580,7 +43581,7 @@
         <v>1.115829446</v>
       </c>
     </row>
-    <row r="313" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>372</v>
       </c>
@@ -50770,7 +50771,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="377" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>383</v>
       </c>
@@ -51150,7 +51151,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="381" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>383</v>
       </c>
@@ -51245,7 +51246,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="382" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>383</v>
       </c>
@@ -51435,7 +51436,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="384" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>383</v>
       </c>
@@ -51815,7 +51816,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="388" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>383</v>
       </c>
@@ -55524,7 +55525,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="423" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>267</v>
       </c>
@@ -55631,7 +55632,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="424" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>267</v>
       </c>
@@ -55738,7 +55739,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="425" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>267</v>
       </c>
@@ -55845,7 +55846,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="426" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>267</v>
       </c>
@@ -68364,7 +68365,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="543" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="543" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A543" t="s">
         <v>282</v>
       </c>
@@ -69006,7 +69007,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="549" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="549" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A549" t="s">
         <v>282</v>
       </c>
@@ -69862,7 +69863,7 @@
         <v>2557</v>
       </c>
     </row>
-    <row r="557" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="557" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A557" t="s">
         <v>372</v>
       </c>
@@ -70183,7 +70184,7 @@
         <v>2557</v>
       </c>
     </row>
-    <row r="560" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="560" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A560" t="s">
         <v>372</v>
       </c>
@@ -77138,7 +77139,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="625" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="625" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A625" t="s">
         <v>295</v>
       </c>
@@ -77352,7 +77353,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="627" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="627" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A627" t="s">
         <v>295</v>
       </c>
@@ -77399,7 +77400,7 @@
         <v>446</v>
       </c>
       <c r="P627">
-        <v>-7.2992700000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="Q627">
         <v>2.189781E-2</v>
@@ -81736,7 +81737,7 @@
         <v>4336</v>
       </c>
     </row>
-    <row r="668" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="668" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A668" t="s">
         <v>207</v>
       </c>
@@ -82057,7 +82058,7 @@
         <v>4336</v>
       </c>
     </row>
-    <row r="671" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="671" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A671" t="s">
         <v>207</v>
       </c>
@@ -82164,7 +82165,7 @@
         <v>4336</v>
       </c>
     </row>
-    <row r="672" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="672" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A672" t="s">
         <v>207</v>
       </c>
@@ -82913,7 +82914,7 @@
         <v>4336</v>
       </c>
     </row>
-    <row r="679" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="679" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A679" t="s">
         <v>207</v>
       </c>
@@ -83448,7 +83449,7 @@
         <v>4336</v>
       </c>
     </row>
-    <row r="684" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="684" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A684" t="s">
         <v>207</v>
       </c>
@@ -83662,7 +83663,7 @@
         <v>4336</v>
       </c>
     </row>
-    <row r="686" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="686" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A686" t="s">
         <v>207</v>
       </c>
@@ -84090,7 +84091,7 @@
         <v>4366</v>
       </c>
     </row>
-    <row r="690" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="690" spans="1:35" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A690" s="7" t="s">
         <v>207</v>
       </c>
@@ -84518,7 +84519,7 @@
         <v>4366</v>
       </c>
     </row>
-    <row r="694" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="694" spans="1:35" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A694" s="7" t="s">
         <v>207</v>
       </c>
@@ -84732,7 +84733,7 @@
         <v>4366</v>
       </c>
     </row>
-    <row r="696" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="696" spans="1:35" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A696" s="7" t="s">
         <v>207</v>
       </c>
@@ -85481,7 +85482,7 @@
         <v>4366</v>
       </c>
     </row>
-    <row r="703" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="703" spans="1:35" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A703" s="7" t="s">
         <v>207</v>
       </c>
@@ -85695,7 +85696,7 @@
         <v>4366</v>
       </c>
     </row>
-    <row r="705" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="705" spans="1:35" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A705" s="7" t="s">
         <v>207</v>
       </c>
@@ -90832,7 +90833,1232 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AR666" xr:uid="{0113C7D2-BE88-4C48-A5D9-9643F889B313}"/>
+  <autoFilter ref="A1:AR752" xr:uid="{0113C7D2-BE88-4C48-A5D9-9643F889B313}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="abundance"/>
+        <filter val="shannon wiener"/>
+        <filter val="taxonomic richness"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="15">
+      <filters>
+        <filter val="0.003694581"/>
+        <filter val="0.00607595"/>
+        <filter val="0.006426735"/>
+        <filter val="0.008928571"/>
+        <filter val="0.009589041"/>
+        <filter val="0.00E+00"/>
+        <filter val="0.016519824"/>
+        <filter val="0.017021277"/>
+        <filter val="0.018493151"/>
+        <filter val="0.01924051"/>
+        <filter val="0.03"/>
+        <filter val="0.030788177"/>
+        <filter val="0.032390746"/>
+        <filter val="0.040773067"/>
+        <filter val="0.044052863"/>
+        <filter val="0.049019608"/>
+        <filter val="0.04964539"/>
+        <filter val="0.05"/>
+        <filter val="0.050108932"/>
+        <filter val="0.05106383"/>
+        <filter val="0.0556962"/>
+        <filter val="0.056041131"/>
+        <filter val="0.056109726"/>
+        <filter val="0.062094763"/>
+        <filter val="0.07"/>
+        <filter val="0.08"/>
+        <filter val="0.082"/>
+        <filter val="0.082119205"/>
+        <filter val="0.09"/>
+        <filter val="0.091106291"/>
+        <filter val="0.099056604"/>
+        <filter val="0.11"/>
+        <filter val="0.111258278"/>
+        <filter val="0.119148936"/>
+        <filter val="0.12"/>
+        <filter val="0.13"/>
+        <filter val="0.135036496"/>
+        <filter val="0.14"/>
+        <filter val="0.1416122"/>
+        <filter val="0.145124717"/>
+        <filter val="0.148601399"/>
+        <filter val="0.15"/>
+        <filter val="0.16"/>
+        <filter val="0.169950739"/>
+        <filter val="0.174876847"/>
+        <filter val="0.18"/>
+        <filter val="0.19"/>
+        <filter val="0.20154185"/>
+        <filter val="0.21"/>
+        <filter val="0.216346154"/>
+        <filter val="0.225770925"/>
+        <filter val="0.22886076"/>
+        <filter val="0.23"/>
+        <filter val="0.24"/>
+        <filter val="0.250896057"/>
+        <filter val="0.26"/>
+        <filter val="0.27"/>
+        <filter val="0.28"/>
+        <filter val="0.3"/>
+        <filter val="0.306382979"/>
+        <filter val="0.30982906"/>
+        <filter val="0.31"/>
+        <filter val="0.33"/>
+        <filter val="0.333774834"/>
+        <filter val="0.334821429"/>
+        <filter val="0.336538462"/>
+        <filter val="0.35"/>
+        <filter val="0.353200883"/>
+        <filter val="0.354"/>
+        <filter val="0.357"/>
+        <filter val="0.36"/>
+        <filter val="0.367132867"/>
+        <filter val="0.37"/>
+        <filter val="0.43"/>
+        <filter val="0.44"/>
+        <filter val="0.45"/>
+        <filter val="0.473372781"/>
+        <filter val="0.478773585"/>
+        <filter val="0.48"/>
+        <filter val="0.485651214"/>
+        <filter val="0.486"/>
+        <filter val="0.5"/>
+        <filter val="0.594713656"/>
+        <filter val="0.6"/>
+        <filter val="0.636042403"/>
+        <filter val="0.650759219"/>
+        <filter val="0.66"/>
+        <filter val="0.67"/>
+        <filter val="0.693430657"/>
+        <filter val="0.7"/>
+        <filter val="0.72"/>
+        <filter val="0.76"/>
+        <filter val="0.79"/>
+        <filter val="0.8"/>
+        <filter val="0.82"/>
+        <filter val="0.83"/>
+        <filter val="0.88"/>
+        <filter val="0.90034965"/>
+        <filter val="0.91"/>
+        <filter val="0.967741935"/>
+        <filter val="0.97"/>
+        <filter val="0.970326409"/>
+        <filter val="1"/>
+        <filter val="1.005882353"/>
+        <filter val="1.01"/>
+        <filter val="1.060070671"/>
+        <filter val="1.063829787"/>
+        <filter val="1.072340426"/>
+        <filter val="1.09"/>
+        <filter val="1.09375"/>
+        <filter val="1.119305857"/>
+        <filter val="1.13"/>
+        <filter val="1.133928571"/>
+        <filter val="1.14"/>
+        <filter val="1.169491525"/>
+        <filter val="1.19"/>
+        <filter val="1.200892857"/>
+        <filter val="1.20149147"/>
+        <filter val="1.203296703"/>
+        <filter val="1.22"/>
+        <filter val="1.24"/>
+        <filter val="1.245762712"/>
+        <filter val="1.25"/>
+        <filter val="1.26"/>
+        <filter val="1.263157895"/>
+        <filter val="1.27"/>
+        <filter val="1.28"/>
+        <filter val="1.31"/>
+        <filter val="1.33"/>
+        <filter val="1.338461538"/>
+        <filter val="1.372377622"/>
+        <filter val="1.379821958"/>
+        <filter val="1.39"/>
+        <filter val="1.392857143"/>
+        <filter val="1.398678414"/>
+        <filter val="1.41"/>
+        <filter val="1.42"/>
+        <filter val="1.43"/>
+        <filter val="1.45"/>
+        <filter val="1.48"/>
+        <filter val="1.48409894"/>
+        <filter val="1.49"/>
+        <filter val="1.506410256"/>
+        <filter val="1.51"/>
+        <filter val="1.515151515"/>
+        <filter val="1.52"/>
+        <filter val="1.54"/>
+        <filter val="1.57"/>
+        <filter val="1.578947368"/>
+        <filter val="1.58"/>
+        <filter val="1.589775561"/>
+        <filter val="1.59"/>
+        <filter val="1.6"/>
+        <filter val="1.720588235"/>
+        <filter val="1.731343284"/>
+        <filter val="1.748251748"/>
+        <filter val="1.759278351"/>
+        <filter val="1.78"/>
+        <filter val="1.83"/>
+        <filter val="1.86"/>
+        <filter val="1.9"/>
+        <filter val="1.93"/>
+        <filter val="1.96"/>
+        <filter val="10"/>
+        <filter val="10.02985075"/>
+        <filter val="10.12048193"/>
+        <filter val="10.13513514"/>
+        <filter val="10.15151515"/>
+        <filter val="10.2"/>
+        <filter val="10.80701754"/>
+        <filter val="10.87719298"/>
+        <filter val="10.96062992"/>
+        <filter val="100"/>
+        <filter val="100.5"/>
+        <filter val="102.1754386"/>
+        <filter val="102.6666667"/>
+        <filter val="104.5643154"/>
+        <filter val="105.5"/>
+        <filter val="107.5"/>
+        <filter val="1089"/>
+        <filter val="11"/>
+        <filter val="11.11842105"/>
+        <filter val="11.36842105"/>
+        <filter val="11.49606299"/>
+        <filter val="11.68421053"/>
+        <filter val="110.5263158"/>
+        <filter val="110.8280255"/>
+        <filter val="111.7021277"/>
+        <filter val="116"/>
+        <filter val="11600"/>
+        <filter val="116182.5726"/>
+        <filter val="118.6246418"/>
+        <filter val="12"/>
+        <filter val="12.25806452"/>
+        <filter val="12.28070175"/>
+        <filter val="12.34939759"/>
+        <filter val="12.60869565"/>
+        <filter val="12.63157895"/>
+        <filter val="12.77192982"/>
+        <filter val="12.98245614"/>
+        <filter val="1206639.004"/>
+        <filter val="12191"/>
+        <filter val="126.6820056"/>
+        <filter val="126.9121813"/>
+        <filter val="1268"/>
+        <filter val="127"/>
+        <filter val="128"/>
+        <filter val="12800"/>
+        <filter val="128223.4957"/>
+        <filter val="13.03030303"/>
+        <filter val="13.23353293"/>
+        <filter val="13.54330709"/>
+        <filter val="13.66666667"/>
+        <filter val="13.73228346"/>
+        <filter val="13100"/>
+        <filter val="131805.1576"/>
+        <filter val="132.3529412"/>
+        <filter val="136103.1519"/>
+        <filter val="138968.4814"/>
+        <filter val="1395.56962"/>
+        <filter val="14"/>
+        <filter val="14.09090909"/>
+        <filter val="14.21686747"/>
+        <filter val="14.23622047"/>
+        <filter val="14.34782609"/>
+        <filter val="14.47098976"/>
+        <filter val="14.84210526"/>
+        <filter val="14.86486486"/>
+        <filter val="14.9"/>
+        <filter val="141.1764706"/>
+        <filter val="1429.411765"/>
+        <filter val="144.4126074"/>
+        <filter val="146.7422096"/>
+        <filter val="147"/>
+        <filter val="1472.590593"/>
+        <filter val="1475.903614"/>
+        <filter val="148.115942"/>
+        <filter val="149.2"/>
+        <filter val="15"/>
+        <filter val="15.234375"/>
+        <filter val="15.33333333"/>
+        <filter val="15.33613445"/>
+        <filter val="15.41516245"/>
+        <filter val="15.5"/>
+        <filter val="15.54054054"/>
+        <filter val="15.56313993"/>
+        <filter val="15.83617747"/>
+        <filter val="153.125"/>
+        <filter val="153.1884058"/>
+        <filter val="1552.795031"/>
+        <filter val="156"/>
+        <filter val="15759.31232"/>
+        <filter val="1585062.241"/>
+        <filter val="159"/>
+        <filter val="159090.9091"/>
+        <filter val="16"/>
+        <filter val="16.1130742"/>
+        <filter val="16.21848739"/>
+        <filter val="16.23188406"/>
+        <filter val="16.41891892"/>
+        <filter val="16.5"/>
+        <filter val="160"/>
+        <filter val="163.0461048"/>
+        <filter val="1689"/>
+        <filter val="169.2650334"/>
+        <filter val="17"/>
+        <filter val="17.27598566"/>
+        <filter val="17.29133858"/>
+        <filter val="17.5"/>
+        <filter val="17.55319149"/>
+        <filter val="17.68421053"/>
+        <filter val="17.88194444"/>
+        <filter val="17.90540541"/>
+        <filter val="170.5382436"/>
+        <filter val="173584.9057"/>
+        <filter val="174"/>
+        <filter val="176.5625"/>
+        <filter val="18"/>
+        <filter val="18.17371938"/>
+        <filter val="18.5"/>
+        <filter val="18.76456876"/>
+        <filter val="182"/>
+        <filter val="1829.268293"/>
+        <filter val="1846"/>
+        <filter val="185.8267717"/>
+        <filter val="186.7021277"/>
+        <filter val="1863.354037"/>
+        <filter val="19"/>
+        <filter val="19.14893617"/>
+        <filter val="19.20547945"/>
+        <filter val="19.31506849"/>
+        <filter val="19.47945205"/>
+        <filter val="19.6563981"/>
+        <filter val="190"/>
+        <filter val="191"/>
+        <filter val="193"/>
+        <filter val="1948"/>
+        <filter val="197.3684211"/>
+        <filter val="197.5103734"/>
+        <filter val="1974"/>
+        <filter val="198.5"/>
+        <filter val="2"/>
+        <filter val="2.04"/>
+        <filter val="2.043269231"/>
+        <filter val="2.088937093"/>
+        <filter val="2.2"/>
+        <filter val="2.217010309"/>
+        <filter val="2.22"/>
+        <filter val="2.245024876"/>
+        <filter val="2.329749104"/>
+        <filter val="2.332155477"/>
+        <filter val="2.35"/>
+        <filter val="2.374545455"/>
+        <filter val="2.4"/>
+        <filter val="2.447761194"/>
+        <filter val="2.52"/>
+        <filter val="2.578125"/>
+        <filter val="2.59"/>
+        <filter val="2.603636364"/>
+        <filter val="2.61"/>
+        <filter val="2.626931567"/>
+        <filter val="2.756183746"/>
+        <filter val="2.89"/>
+        <filter val="2.916666667"/>
+        <filter val="2.93"/>
+        <filter val="2.94"/>
+        <filter val="2.955188679"/>
+        <filter val="2.980769231"/>
+        <filter val="20.68493151"/>
+        <filter val="20.74468085"/>
+        <filter val="20.98939929"/>
+        <filter val="200"/>
+        <filter val="2031"/>
+        <filter val="2073.170732"/>
+        <filter val="2084.33735"/>
+        <filter val="21"/>
+        <filter val="21.5625"/>
+        <filter val="21.78217822"/>
+        <filter val="2100"/>
+        <filter val="2121.95122"/>
+        <filter val="216.86747"/>
+        <filter val="22.16438356"/>
+        <filter val="22.43835616"/>
+        <filter val="2201.183432"/>
+        <filter val="223"/>
+        <filter val="2251.552795"/>
+        <filter val="228"/>
+        <filter val="228.125"/>
+        <filter val="23"/>
+        <filter val="23.64864865"/>
+        <filter val="23.671875"/>
+        <filter val="23.7"/>
+        <filter val="23.93617021"/>
+        <filter val="231.4285714"/>
+        <filter val="232098.7654"/>
+        <filter val="2372.262774"/>
+        <filter val="24.13793103"/>
+        <filter val="24.21686747"/>
+        <filter val="24.5"/>
+        <filter val="24.57337884"/>
+        <filter val="24.59770115"/>
+        <filter val="24.66666667"/>
+        <filter val="24.83870968"/>
+        <filter val="24.91803279"/>
+        <filter val="243"/>
+        <filter val="244"/>
+        <filter val="25"/>
+        <filter val="2536.585366"/>
+        <filter val="25659.82405"/>
+        <filter val="26.03508772"/>
+        <filter val="26.2"/>
+        <filter val="26.45879733"/>
+        <filter val="26.66666667"/>
+        <filter val="26.7"/>
+        <filter val="260.8"/>
+        <filter val="261635.2201"/>
+        <filter val="265.8227848"/>
+        <filter val="266"/>
+        <filter val="27"/>
+        <filter val="27.24137931"/>
+        <filter val="27.33333333"/>
+        <filter val="27.36486486"/>
+        <filter val="27.77385159"/>
+        <filter val="27.91666667"/>
+        <filter val="279.6"/>
+        <filter val="28.37837838"/>
+        <filter val="2802.21519"/>
+        <filter val="282.3529412"/>
+        <filter val="283.0434783"/>
+        <filter val="287.9746835"/>
+        <filter val="289.5184136"/>
+        <filter val="29"/>
+        <filter val="29.296875"/>
+        <filter val="29.375"/>
+        <filter val="29.4"/>
+        <filter val="29.72972973"/>
+        <filter val="3"/>
+        <filter val="3.003412969"/>
+        <filter val="3.13"/>
+        <filter val="3.214545455"/>
+        <filter val="3.235294118"/>
+        <filter val="3.3"/>
+        <filter val="3.35"/>
+        <filter val="3.42"/>
+        <filter val="3.47826087"/>
+        <filter val="3.5"/>
+        <filter val="3.555555556"/>
+        <filter val="3.620071685"/>
+        <filter val="3.66509434"/>
+        <filter val="3.789473684"/>
+        <filter val="3.8"/>
+        <filter val="3.919821826"/>
+        <filter val="30"/>
+        <filter val="30.06756757"/>
+        <filter val="30791.78886"/>
+        <filter val="31.20567376"/>
+        <filter val="31.43859649"/>
+        <filter val="31.91489362"/>
+        <filter val="3105.590062"/>
+        <filter val="31446.54088"/>
+        <filter val="317.0731707"/>
+        <filter val="317.6470588"/>
+        <filter val="317000"/>
+        <filter val="32"/>
+        <filter val="32.09459459"/>
+        <filter val="32.5"/>
+        <filter val="32.69461078"/>
+        <filter val="325.3012048"/>
+        <filter val="3300"/>
+        <filter val="3333"/>
+        <filter val="337.349398"/>
+        <filter val="34.03614458"/>
+        <filter val="34.55830389"/>
+        <filter val="3416.149068"/>
+        <filter val="35.54166667"/>
+        <filter val="3555"/>
+        <filter val="36"/>
+        <filter val="36.48"/>
+        <filter val="36.6255144"/>
+        <filter val="36.86868687"/>
+        <filter val="367.9245283"/>
+        <filter val="37"/>
+        <filter val="37.9"/>
+        <filter val="37249.28367"/>
+        <filter val="373.493976"/>
+        <filter val="37338"/>
+        <filter val="38"/>
+        <filter val="380.3067152"/>
+        <filter val="38123.16716"/>
+        <filter val="389.3129771"/>
+        <filter val="38929"/>
+        <filter val="39.18918919"/>
+        <filter val="39.3"/>
+        <filter val="39.4"/>
+        <filter val="39.7005988"/>
+        <filter val="392"/>
+        <filter val="4"/>
+        <filter val="4.00E+05"/>
+        <filter val="4.071428571"/>
+        <filter val="4.105263158"/>
+        <filter val="4.13"/>
+        <filter val="4.166666667"/>
+        <filter val="4.2"/>
+        <filter val="4.210526316"/>
+        <filter val="4.232727273"/>
+        <filter val="4.243697479"/>
+        <filter val="4.34"/>
+        <filter val="4.4"/>
+        <filter val="4.421052632"/>
+        <filter val="4.462585034"/>
+        <filter val="4.478672986"/>
+        <filter val="4.480286738"/>
+        <filter val="4.5"/>
+        <filter val="4.527972028"/>
+        <filter val="4.64"/>
+        <filter val="4.657836645"/>
+        <filter val="4.664310954"/>
+        <filter val="4.74789916"/>
+        <filter val="4.8"/>
+        <filter val="40.8"/>
+        <filter val="41"/>
+        <filter val="41200"/>
+        <filter val="416.4305949"/>
+        <filter val="42.01149425"/>
+        <filter val="42.5"/>
+        <filter val="42.6035503"/>
+        <filter val="42.8668942"/>
+        <filter val="43.91891892"/>
+        <filter val="434.2"/>
+        <filter val="436.2606232"/>
+        <filter val="44.1"/>
+        <filter val="44.93243243"/>
+        <filter val="4422"/>
+        <filter val="46"/>
+        <filter val="468"/>
+        <filter val="47"/>
+        <filter val="47239"/>
+        <filter val="4898"/>
+        <filter val="49.04215602"/>
+        <filter val="5"/>
+        <filter val="5.127610209"/>
+        <filter val="5.307692308"/>
+        <filter val="5.419354839"/>
+        <filter val="5.512367491"/>
+        <filter val="5.52"/>
+        <filter val="5.555555556"/>
+        <filter val="5.58"/>
+        <filter val="5.632727273"/>
+        <filter val="5.684210526"/>
+        <filter val="5.724381625"/>
+        <filter val="5.93639576"/>
+        <filter val="509.375"/>
+        <filter val="51.35135135"/>
+        <filter val="52.5"/>
+        <filter val="53.04054054"/>
+        <filter val="53.47826087"/>
+        <filter val="538.2352941"/>
+        <filter val="54"/>
+        <filter val="55.3125"/>
+        <filter val="55.40540541"/>
+        <filter val="553086.4198"/>
+        <filter val="56.56565657"/>
+        <filter val="57.27810651"/>
+        <filter val="572"/>
+        <filter val="578.313253"/>
+        <filter val="589.7550111"/>
+        <filter val="59800"/>
+        <filter val="6"/>
+        <filter val="6.013513514"/>
+        <filter val="6.060606061"/>
+        <filter val="6.166666667"/>
+        <filter val="6.2"/>
+        <filter val="6.231884058"/>
+        <filter val="6.462053841"/>
+        <filter val="6.498442368"/>
+        <filter val="6.5"/>
+        <filter val="6.523297491"/>
+        <filter val="6.542056075"/>
+        <filter val="6.625"/>
+        <filter val="6.784386617"/>
+        <filter val="6.86440678"/>
+        <filter val="6.956521739"/>
+        <filter val="60.9375"/>
+        <filter val="60850.43988"/>
+        <filter val="61.48648649"/>
+        <filter val="61.89111748"/>
+        <filter val="624"/>
+        <filter val="63"/>
+        <filter val="630"/>
+        <filter val="64"/>
+        <filter val="64.0625"/>
+        <filter val="64.5"/>
+        <filter val="65249.26686"/>
+        <filter val="66000"/>
+        <filter val="662.650602"/>
+        <filter val="668.6746988"/>
+        <filter val="674"/>
+        <filter val="682.9268293"/>
+        <filter val="685.8238559"/>
+        <filter val="6850"/>
+        <filter val="69.26315789"/>
+        <filter val="69.70954357"/>
+        <filter val="69484.24069"/>
+        <filter val="7"/>
+        <filter val="7.021806854"/>
+        <filter val="7.086092715"/>
+        <filter val="7.161290323"/>
+        <filter val="7.208480565"/>
+        <filter val="7.368421053"/>
+        <filter val="7.458333333"/>
+        <filter val="7.536231884"/>
+        <filter val="7.763239875"/>
+        <filter val="70.55084746"/>
+        <filter val="70200"/>
+        <filter val="71.68141593"/>
+        <filter val="710"/>
+        <filter val="713.9718956"/>
+        <filter val="72.8"/>
+        <filter val="73"/>
+        <filter val="73.04347826"/>
+        <filter val="7375.776398"/>
+        <filter val="76.61469933"/>
+        <filter val="7763.975155"/>
+        <filter val="780.4878049"/>
+        <filter val="79.7979798"/>
+        <filter val="7990"/>
+        <filter val="8"/>
+        <filter val="8.043478261"/>
+        <filter val="8.056537102"/>
+        <filter val="8.080808081"/>
+        <filter val="8.129032258"/>
+        <filter val="8.151260504"/>
+        <filter val="8.25"/>
+        <filter val="8.46105919"/>
+        <filter val="8.53E-14"/>
+        <filter val="8.550724638"/>
+        <filter val="8.6"/>
+        <filter val="8.722741433"/>
+        <filter val="8.730512249"/>
+        <filter val="8.782287823"/>
+        <filter val="8.90459364"/>
+        <filter val="8064.516129"/>
+        <filter val="82.9787234"/>
+        <filter val="8211.206897"/>
+        <filter val="83.8"/>
+        <filter val="830.6962025"/>
+        <filter val="839"/>
+        <filter val="861.9402985"/>
+        <filter val="87"/>
+        <filter val="87.5"/>
+        <filter val="87.65625"/>
+        <filter val="88"/>
+        <filter val="88.23529412"/>
+        <filter val="88.42105263"/>
+        <filter val="88.88888889"/>
+        <filter val="89.36170213"/>
+        <filter val="890"/>
+        <filter val="9"/>
+        <filter val="9.04400257"/>
+        <filter val="9.159663866"/>
+        <filter val="9.551401869"/>
+        <filter val="9.565217391"/>
+        <filter val="9.6"/>
+        <filter val="9.731343284"/>
+        <filter val="9.78"/>
+        <filter val="9.797297297"/>
+        <filter val="9.964664311"/>
+        <filter val="90.83333333"/>
+        <filter val="91.21813031"/>
+        <filter val="927.710843"/>
+        <filter val="95"/>
+        <filter val="97.05882353"/>
+        <filter val="97400"/>
+        <filter val="99.15014164"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="16">
+      <filters>
+        <filter val="0.002739726"/>
+        <filter val="0.003084833"/>
+        <filter val="0.003303965"/>
+        <filter val="0.008510638"/>
+        <filter val="0.00862069"/>
+        <filter val="0.009113924"/>
+        <filter val="0.027763496"/>
+        <filter val="0.03"/>
+        <filter val="0.03553616"/>
+        <filter val="0.035761589"/>
+        <filter val="0.03630137"/>
+        <filter val="0.04"/>
+        <filter val="0.04679803"/>
+        <filter val="0.048586118"/>
+        <filter val="0.05"/>
+        <filter val="0.05106383"/>
+        <filter val="0.055361596"/>
+        <filter val="0.06"/>
+        <filter val="0.065359477"/>
+        <filter val="0.066964286"/>
+        <filter val="0.071585903"/>
+        <filter val="0.072260274"/>
+        <filter val="0.072340426"/>
+        <filter val="0.08"/>
+        <filter val="0.088669951"/>
+        <filter val="0.09"/>
+        <filter val="0.094177215"/>
+        <filter val="0.099056604"/>
+        <filter val="0.11"/>
+        <filter val="0.110132159"/>
+        <filter val="0.111607143"/>
+        <filter val="0.12"/>
+        <filter val="0.13"/>
+        <filter val="0.130922693"/>
+        <filter val="0.139433551"/>
+        <filter val="0.14"/>
+        <filter val="0.143171806"/>
+        <filter val="0.15"/>
+        <filter val="0.156182213"/>
+        <filter val="0.157635468"/>
+        <filter val="0.16"/>
+        <filter val="0.163265306"/>
+        <filter val="0.17"/>
+        <filter val="0.171532847"/>
+        <filter val="0.174825175"/>
+        <filter val="0.18"/>
+        <filter val="0.188325991"/>
+        <filter val="0.19"/>
+        <filter val="0.2"/>
+        <filter val="0.21"/>
+        <filter val="0.221132898"/>
+        <filter val="0.23"/>
+        <filter val="0.240384615"/>
+        <filter val="0.259602649"/>
+        <filter val="0.26"/>
+        <filter val="0.262278481"/>
+        <filter val="0.27"/>
+        <filter val="0.286738351"/>
+        <filter val="0.287417219"/>
+        <filter val="0.3"/>
+        <filter val="0.32"/>
+        <filter val="0.33"/>
+        <filter val="0.331125828"/>
+        <filter val="0.34"/>
+        <filter val="0.34965035"/>
+        <filter val="0.351"/>
+        <filter val="0.35177305"/>
+        <filter val="0.357905983"/>
+        <filter val="0.36"/>
+        <filter val="0.37"/>
+        <filter val="0.38"/>
+        <filter val="0.4"/>
+        <filter val="0.402"/>
+        <filter val="0.41"/>
+        <filter val="0.429501085"/>
+        <filter val="0.44"/>
+        <filter val="0.447"/>
+        <filter val="0.46"/>
+        <filter val="0.462264151"/>
+        <filter val="0.483"/>
+        <filter val="0.49787234"/>
+        <filter val="0.5"/>
+        <filter val="0.51"/>
+        <filter val="0.54"/>
+        <filter val="0.55"/>
+        <filter val="0.551094891"/>
+        <filter val="0.57"/>
+        <filter val="0.6"/>
+        <filter val="0.62"/>
+        <filter val="0.64"/>
+        <filter val="0.649038462"/>
+        <filter val="0.66"/>
+        <filter val="0.684326711"/>
+        <filter val="0.7"/>
+        <filter val="0.75"/>
+        <filter val="0.791208791"/>
+        <filter val="0.8"/>
+        <filter val="0.805084746"/>
+        <filter val="0.81"/>
+        <filter val="0.811764706"/>
+        <filter val="0.82"/>
+        <filter val="0.83"/>
+        <filter val="0.833333333"/>
+        <filter val="0.84"/>
+        <filter val="0.86"/>
+        <filter val="0.863501484"/>
+        <filter val="0.870967742"/>
+        <filter val="0.88"/>
+        <filter val="0.906593407"/>
+        <filter val="0.943600868"/>
+        <filter val="0.945512821"/>
+        <filter val="0.946745562"/>
+        <filter val="0.96"/>
+        <filter val="1"/>
+        <filter val="1.008510638"/>
+        <filter val="1.02"/>
+        <filter val="1.025423729"/>
+        <filter val="1.03"/>
+        <filter val="1.063829787"/>
+        <filter val="1.091022444"/>
+        <filter val="1.1"/>
+        <filter val="1.107692308"/>
+        <filter val="1.13"/>
+        <filter val="1.217647059"/>
+        <filter val="1.22"/>
+        <filter val="1.236607143"/>
+        <filter val="1.237388724"/>
+        <filter val="1.31"/>
+        <filter val="1.33"/>
+        <filter val="1.351351351"/>
+        <filter val="1.38"/>
+        <filter val="1.42"/>
+        <filter val="1.44249147"/>
+        <filter val="1.48"/>
+        <filter val="1.482142857"/>
+        <filter val="1.5"/>
+        <filter val="1.51"/>
+        <filter val="1.53"/>
+        <filter val="1.541218638"/>
+        <filter val="1.55"/>
+        <filter val="1.555944056"/>
+        <filter val="1.58"/>
+        <filter val="1.6"/>
+        <filter val="1.689189189"/>
+        <filter val="1.696035242"/>
+        <filter val="1.76"/>
+        <filter val="1.77"/>
+        <filter val="1.81"/>
+        <filter val="1.814948454"/>
+        <filter val="1.816494845"/>
+        <filter val="1.85"/>
+        <filter val="1.88"/>
+        <filter val="1.91"/>
+        <filter val="1.930927835"/>
+        <filter val="1.94"/>
+        <filter val="1.96"/>
+        <filter val="1.98"/>
+        <filter val="1.99"/>
+        <filter val="1.99132321"/>
+        <filter val="10.08333333"/>
+        <filter val="10.10526316"/>
+        <filter val="10.16806723"/>
+        <filter val="10.6"/>
+        <filter val="10.66666667"/>
+        <filter val="10.68535826"/>
+        <filter val="10.81081081"/>
+        <filter val="10.84507042"/>
+        <filter val="10.86956522"/>
+        <filter val="100"/>
+        <filter val="102"/>
+        <filter val="104.8728814"/>
+        <filter val="105.6521739"/>
+        <filter val="105.730659"/>
+        <filter val="107.082153"/>
+        <filter val="11"/>
+        <filter val="11.33802817"/>
+        <filter val="11.87279152"/>
+        <filter val="110.9375"/>
+        <filter val="1109.56164"/>
+        <filter val="1118.670886"/>
+        <filter val="114.7058824"/>
+        <filter val="11645.96273"/>
+        <filter val="118035.1906"/>
+        <filter val="1194"/>
+        <filter val="119627.5072"/>
+        <filter val="12"/>
+        <filter val="12.41935484"/>
+        <filter val="12.63157895"/>
+        <filter val="12.72084806"/>
+        <filter val="12.75362319"/>
+        <filter val="12.83783784"/>
+        <filter val="12.94736842"/>
+        <filter val="12.95180723"/>
+        <filter val="120343.8395"/>
+        <filter val="121.2765957"/>
+        <filter val="1216.86747"/>
+        <filter val="1219753.086"/>
+        <filter val="122"/>
+        <filter val="122.8723404"/>
+        <filter val="1263"/>
+        <filter val="1269"/>
+        <filter val="128.6884632"/>
+        <filter val="13.125"/>
+        <filter val="13.3744856"/>
+        <filter val="13.62275449"/>
+        <filter val="13.63636364"/>
+        <filter val="13.95275591"/>
+        <filter val="131805.1576"/>
+        <filter val="133333.3333"/>
+        <filter val="134"/>
+        <filter val="1349.39759"/>
+        <filter val="13600"/>
+        <filter val="1364"/>
+        <filter val="14.04166667"/>
+        <filter val="14.18918919"/>
+        <filter val="14.58333333"/>
+        <filter val="14.72891566"/>
+        <filter val="14.74015748"/>
+        <filter val="14.78873239"/>
+        <filter val="14.8409894"/>
+        <filter val="14.95798319"/>
+        <filter val="14.96062992"/>
+        <filter val="14.99099721"/>
+        <filter val="141.0144928"/>
+        <filter val="143"/>
+        <filter val="147"/>
+        <filter val="1497"/>
+        <filter val="15"/>
+        <filter val="15.5"/>
+        <filter val="15.52755906"/>
+        <filter val="15.87837838"/>
+        <filter val="150"/>
+        <filter val="16.01694915"/>
+        <filter val="16.09318996"/>
+        <filter val="16.30289532"/>
+        <filter val="16.37681159"/>
+        <filter val="16.55405405"/>
+        <filter val="16.66666667"/>
+        <filter val="16.76056338"/>
+        <filter val="16.7605634"/>
+        <filter val="16.89189189"/>
+        <filter val="16.92650334"/>
+        <filter val="1605.839416"/>
+        <filter val="162"/>
+        <filter val="1638.554217"/>
+        <filter val="17"/>
+        <filter val="17.33333333"/>
+        <filter val="170.5382436"/>
+        <filter val="178.4"/>
+        <filter val="179.3"/>
+        <filter val="179799.4269"/>
+        <filter val="18"/>
+        <filter val="18.1092437"/>
+        <filter val="18.58333333"/>
+        <filter val="18.91891892"/>
+        <filter val="182.4362606"/>
+        <filter val="182716.0494"/>
+        <filter val="18322.98137"/>
+        <filter val="185892.1162"/>
+        <filter val="186"/>
+        <filter val="187.0824053"/>
+        <filter val="19"/>
+        <filter val="19.35483871"/>
+        <filter val="19.59459459"/>
+        <filter val="1905"/>
+        <filter val="191"/>
+        <filter val="194"/>
+        <filter val="194.7"/>
+        <filter val="2"/>
+        <filter val="2.02"/>
+        <filter val="2.1"/>
+        <filter val="2.12"/>
+        <filter val="2.185314685"/>
+        <filter val="2.1875"/>
+        <filter val="2.2"/>
+        <filter val="2.3"/>
+        <filter val="2.374545455"/>
+        <filter val="2.4"/>
+        <filter val="2.44"/>
+        <filter val="2.46"/>
+        <filter val="2.493781095"/>
+        <filter val="2.503401361"/>
+        <filter val="2.55"/>
+        <filter val="2.603636364"/>
+        <filter val="2.66"/>
+        <filter val="2.76169265"/>
+        <filter val="2.78125"/>
+        <filter val="2.83"/>
+        <filter val="20.33333333"/>
+        <filter val="20.5"/>
+        <filter val="20.72463768"/>
+        <filter val="20.91954023"/>
+        <filter val="21"/>
+        <filter val="21.3"/>
+        <filter val="21.5"/>
+        <filter val="210.1983003"/>
+        <filter val="2121.95122"/>
+        <filter val="2153.846154"/>
+        <filter val="216.0444157"/>
+        <filter val="22"/>
+        <filter val="22.03065134"/>
+        <filter val="22.265625"/>
+        <filter val="22.6"/>
+        <filter val="220"/>
+        <filter val="220000"/>
+        <filter val="2208"/>
+        <filter val="229.4117647"/>
+        <filter val="23"/>
+        <filter val="23.04964539"/>
+        <filter val="23.18181818"/>
+        <filter val="23.31081081"/>
+        <filter val="23.5"/>
+        <filter val="23.6"/>
+        <filter val="23.64864865"/>
+        <filter val="23.671875"/>
+        <filter val="231446.5409"/>
+        <filter val="232.5949367"/>
+        <filter val="2390.243902"/>
+        <filter val="24"/>
+        <filter val="24.1917808"/>
+        <filter val="24.32432432"/>
+        <filter val="24.5"/>
+        <filter val="24.9122807"/>
+        <filter val="2487.951807"/>
+        <filter val="25.2"/>
+        <filter val="25.4520548"/>
+        <filter val="25.53191489"/>
+        <filter val="25.60240964"/>
+        <filter val="25.66552901"/>
+        <filter val="25.7260274"/>
+        <filter val="25.78125"/>
+        <filter val="25.90361446"/>
+        <filter val="2560.97561"/>
+        <filter val="257.1428571"/>
+        <filter val="26"/>
+        <filter val="26.1643836"/>
+        <filter val="26.26262626"/>
+        <filter val="260.8"/>
+        <filter val="2602.848101"/>
+        <filter val="265.7223796"/>
+        <filter val="27.08333333"/>
+        <filter val="27.12765957"/>
+        <filter val="27.1875"/>
+        <filter val="271.7668922"/>
+        <filter val="272"/>
+        <filter val="277.1084337"/>
+        <filter val="28.72340426"/>
+        <filter val="287.3134328"/>
+        <filter val="29.04564315"/>
+        <filter val="29.7"/>
+        <filter val="292.1052632"/>
+        <filter val="29635"/>
+        <filter val="298.4375"/>
+        <filter val="299"/>
+        <filter val="3"/>
+        <filter val="3.024475524"/>
+        <filter val="3.044776119"/>
+        <filter val="3.083900227"/>
+        <filter val="3.164179104"/>
+        <filter val="3.18"/>
+        <filter val="3.2"/>
+        <filter val="3.21"/>
+        <filter val="3.214545455"/>
+        <filter val="3.27"/>
+        <filter val="3.3"/>
+        <filter val="3.369230769"/>
+        <filter val="3.4"/>
+        <filter val="3.400473934"/>
+        <filter val="3.411552347"/>
+        <filter val="3.5"/>
+        <filter val="3.542435424"/>
+        <filter val="3.7"/>
+        <filter val="3.76344086"/>
+        <filter val="3.839285714"/>
+        <filter val="3.942307692"/>
+        <filter val="30"/>
+        <filter val="30.06756757"/>
+        <filter val="30.45454545"/>
+        <filter val="307.8838174"/>
+        <filter val="308.8235294"/>
+        <filter val="31"/>
+        <filter val="31.33333333"/>
+        <filter val="3119"/>
+        <filter val="315.3674833"/>
+        <filter val="318.0467091"/>
+        <filter val="32"/>
+        <filter val="32.30538922"/>
+        <filter val="326.4705882"/>
+        <filter val="327"/>
+        <filter val="33"/>
+        <filter val="33.44594595"/>
+        <filter val="33.515625"/>
+        <filter val="3341.463415"/>
+        <filter val="33724.34018"/>
+        <filter val="340.625"/>
+        <filter val="343.3544304"/>
+        <filter val="34457.47801"/>
+        <filter val="347.8723404"/>
+        <filter val="35.04"/>
+        <filter val="35.33333333"/>
+        <filter val="35.41916168"/>
+        <filter val="35.50295858"/>
+        <filter val="358.4527221"/>
+        <filter val="36.52173913"/>
+        <filter val="36.7"/>
+        <filter val="362.2641509"/>
+        <filter val="36600"/>
+        <filter val="372.8045326"/>
+        <filter val="378.125"/>
+        <filter val="38.3"/>
+        <filter val="38.9"/>
+        <filter val="38000"/>
+        <filter val="385"/>
+        <filter val="389.0183004"/>
+        <filter val="39.65034965"/>
+        <filter val="39.8989899"/>
+        <filter val="39100"/>
+        <filter val="3975.609756"/>
+        <filter val="4.054054054"/>
+        <filter val="4.077830189"/>
+        <filter val="4.094339623"/>
+        <filter val="4.232727273"/>
+        <filter val="4.4"/>
+        <filter val="4.42"/>
+        <filter val="4.436619718"/>
+        <filter val="4.459459459"/>
+        <filter val="4.5"/>
+        <filter val="4.52173913"/>
+        <filter val="4.64"/>
+        <filter val="4.8"/>
+        <filter val="4.802867384"/>
+        <filter val="4.869565217"/>
+        <filter val="4.92957746"/>
+        <filter val="40"/>
+        <filter val="40.23668639"/>
+        <filter val="40.70175439"/>
+        <filter val="40.8"/>
+        <filter val="4012"/>
+        <filter val="41.7"/>
+        <filter val="414"/>
+        <filter val="42.88732394"/>
+        <filter val="43.08510638"/>
+        <filter val="43.66666667"/>
+        <filter val="434.2"/>
+        <filter val="438.0952381"/>
+        <filter val="44.16666667"/>
+        <filter val="44341"/>
+        <filter val="458.9211618"/>
+        <filter val="46"/>
+        <filter val="46.21908127"/>
+        <filter val="46.5"/>
+        <filter val="46.79166667"/>
+        <filter val="463.4146341"/>
+        <filter val="47.81690141"/>
+        <filter val="479.8866856"/>
+        <filter val="485.4961832"/>
+        <filter val="485.9375"/>
+        <filter val="495.3125"/>
+        <filter val="5"/>
+        <filter val="5.06"/>
+        <filter val="5.067567568"/>
+        <filter val="5.148514851"/>
+        <filter val="5.263157895"/>
+        <filter val="5.368421053"/>
+        <filter val="5.496688742"/>
+        <filter val="5.504201681"/>
+        <filter val="5.576208178"/>
+        <filter val="5.591397849"/>
+        <filter val="5.632727273"/>
+        <filter val="5.652173913"/>
+        <filter val="5.743243243"/>
+        <filter val="5.93639576"/>
+        <filter val="503703.7037"/>
+        <filter val="50586.51026"/>
+        <filter val="506.0240964"/>
+        <filter val="51380"/>
+        <filter val="52.65957447"/>
+        <filter val="53.7883959"/>
+        <filter val="54.7826087"/>
+        <filter val="542.1686747"/>
+        <filter val="55"/>
+        <filter val="55.95628415"/>
+        <filter val="554.2168675"/>
+        <filter val="559.4654788"/>
+        <filter val="56.66666667"/>
+        <filter val="563"/>
+        <filter val="5678"/>
+        <filter val="5730"/>
+        <filter val="59.7"/>
+        <filter val="5916"/>
+        <filter val="6"/>
+        <filter val="6.026490066"/>
+        <filter val="6.060606061"/>
+        <filter val="6.125"/>
+        <filter val="6.203090508"/>
+        <filter val="6.416666667"/>
+        <filter val="6.5"/>
+        <filter val="6.548387097"/>
+        <filter val="6.682134571"/>
+        <filter val="6.754261364"/>
+        <filter val="6.756756757"/>
+        <filter val="6.774193548"/>
+        <filter val="6.8"/>
+        <filter val="6.89"/>
+        <filter val="6.901408451"/>
+        <filter val="60"/>
+        <filter val="61.7"/>
+        <filter val="614.4578313"/>
+        <filter val="62.34375"/>
+        <filter val="62.6056338"/>
+        <filter val="64"/>
+        <filter val="65.78313253"/>
+        <filter val="65.80204778"/>
+        <filter val="659.0509805"/>
+        <filter val="67.57894737"/>
+        <filter val="67.91666667"/>
+        <filter val="69.01408451"/>
+        <filter val="698755.1867"/>
+        <filter val="7"/>
+        <filter val="7.094594595"/>
+        <filter val="7.142857143"/>
+        <filter val="7.263157895"/>
+        <filter val="7.272727273"/>
+        <filter val="7.395104895"/>
+        <filter val="7.575757576"/>
+        <filter val="7.971014493"/>
+        <filter val="70"/>
+        <filter val="704.8192771"/>
+        <filter val="7047.413793"/>
+        <filter val="710.8433735"/>
+        <filter val="7400"/>
+        <filter val="7453.416149"/>
+        <filter val="7547.169811"/>
+        <filter val="76.76767677"/>
+        <filter val="7608.695652"/>
+        <filter val="767.6470588"/>
+        <filter val="78"/>
+        <filter val="79.6460177"/>
+        <filter val="8"/>
+        <filter val="8.056537102"/>
+        <filter val="8.322580645"/>
+        <filter val="8.355263158"/>
+        <filter val="8.403361345"/>
+        <filter val="8.446153846"/>
+        <filter val="8.529411765"/>
+        <filter val="8.6"/>
+        <filter val="8.722741433"/>
+        <filter val="8.771929825"/>
+        <filter val="8.955223881"/>
+        <filter val="800"/>
+        <filter val="827.7936963"/>
+        <filter val="84.57446809"/>
+        <filter val="853.6585366"/>
+        <filter val="86.36363636"/>
+        <filter val="860"/>
+        <filter val="884"/>
+        <filter val="892946.0581"/>
+        <filter val="9"/>
+        <filter val="9.12"/>
+        <filter val="9.157894737"/>
+        <filter val="9.175946548"/>
+        <filter val="9.333333333"/>
+        <filter val="9.454976303"/>
+        <filter val="9.473684211"/>
+        <filter val="9.552238806"/>
+        <filter val="9.6"/>
+        <filter val="9.710144928"/>
+        <filter val="9.78"/>
+        <filter val="908.2278481"/>
+        <filter val="911"/>
+        <filter val="923"/>
+        <filter val="926.4705882"/>
+        <filter val="93300"/>
+        <filter val="974"/>
+        <filter val="98"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">

</xml_diff>

<commit_message>
lots of tweaks to data
</commit_message>
<xml_diff>
--- a/data/data_extraction.xlsx
+++ b/data/data_extraction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\work\Projects\In_progress\precip_changes_soil_fauna\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4AE8968-9A73-413F-A34A-0E74DDA74732}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1A1C58-DA1B-477E-81C1-80171D336910}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="articles" sheetId="1" r:id="rId1"/>
@@ -3798,7 +3798,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55AD3176-A41F-4F7C-892D-39B873D09377}">
   <dimension ref="A1:V47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="U46" sqref="U46"/>
@@ -7030,9 +7030,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AR752"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P753" sqref="P753"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A636" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AI747" sqref="AI747"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14295,7 +14295,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="64" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>295</v>
       </c>
@@ -14884,7 +14884,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="69" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>295</v>
       </c>
@@ -52101,7 +52101,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="391" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>369</v>
       </c>
@@ -52208,7 +52208,7 @@
         <v>3590</v>
       </c>
     </row>
-    <row r="392" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>369</v>
       </c>
@@ -52315,7 +52315,7 @@
         <v>3590</v>
       </c>
     </row>
-    <row r="393" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>316</v>
       </c>
@@ -52422,7 +52422,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="394" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>316</v>
       </c>
@@ -52529,7 +52529,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="395" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>316</v>
       </c>
@@ -52636,7 +52636,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="396" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>316</v>
       </c>
@@ -52743,7 +52743,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="397" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>316</v>
       </c>
@@ -52850,7 +52850,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="398" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>316</v>
       </c>
@@ -52957,7 +52957,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="399" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>316</v>
       </c>
@@ -53064,7 +53064,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="400" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:36" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>316</v>
       </c>
@@ -53171,7 +53171,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="401" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>316</v>
       </c>
@@ -53278,7 +53278,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="402" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>316</v>
       </c>
@@ -53385,7 +53385,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="403" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>316</v>
       </c>
@@ -53492,7 +53492,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="404" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>316</v>
       </c>
@@ -53599,7 +53599,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="405" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>316</v>
       </c>
@@ -53706,7 +53706,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="406" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>316</v>
       </c>
@@ -53813,7 +53813,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="407" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>316</v>
       </c>
@@ -53920,7 +53920,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="408" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>316</v>
       </c>
@@ -54027,7 +54027,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="409" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>316</v>
       </c>
@@ -54134,7 +54134,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="410" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>316</v>
       </c>
@@ -54241,7 +54241,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="411" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>316</v>
       </c>
@@ -54348,7 +54348,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="412" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>316</v>
       </c>
@@ -54455,7 +54455,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="413" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>316</v>
       </c>
@@ -54562,7 +54562,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="414" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>316</v>
       </c>
@@ -54669,7 +54669,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="415" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>316</v>
       </c>
@@ -54776,7 +54776,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="416" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>316</v>
       </c>
@@ -54883,7 +54883,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="417" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>316</v>
       </c>
@@ -54990,7 +54990,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="418" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>316</v>
       </c>
@@ -55097,7 +55097,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="419" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>316</v>
       </c>
@@ -55204,7 +55204,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="420" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>316</v>
       </c>
@@ -55311,7 +55311,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="421" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>316</v>
       </c>
@@ -55418,7 +55418,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="422" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>316</v>
       </c>
@@ -55953,7 +55953,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="427" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>357</v>
       </c>
@@ -56060,7 +56060,7 @@
         <v>2190</v>
       </c>
     </row>
-    <row r="428" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>357</v>
       </c>
@@ -56167,7 +56167,7 @@
         <v>2190</v>
       </c>
     </row>
-    <row r="429" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>357</v>
       </c>
@@ -56274,7 +56274,7 @@
         <v>2190</v>
       </c>
     </row>
-    <row r="430" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>357</v>
       </c>
@@ -56381,7 +56381,7 @@
         <v>2190</v>
       </c>
     </row>
-    <row r="431" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>333</v>
       </c>
@@ -56488,7 +56488,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="432" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>333</v>
       </c>
@@ -56595,7 +56595,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="433" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
         <v>333</v>
       </c>
@@ -56702,7 +56702,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="434" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
         <v>333</v>
       </c>
@@ -56809,7 +56809,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="435" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
         <v>333</v>
       </c>
@@ -56916,7 +56916,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="436" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>333</v>
       </c>
@@ -57023,7 +57023,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="437" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
         <v>333</v>
       </c>
@@ -57130,7 +57130,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="438" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
         <v>333</v>
       </c>
@@ -57237,7 +57237,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="439" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
         <v>333</v>
       </c>
@@ -57344,7 +57344,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="440" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
         <v>333</v>
       </c>
@@ -57451,7 +57451,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="441" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
         <v>333</v>
       </c>
@@ -57558,7 +57558,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="442" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
         <v>333</v>
       </c>
@@ -57665,7 +57665,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="443" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
         <v>333</v>
       </c>
@@ -57772,7 +57772,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="444" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
         <v>333</v>
       </c>
@@ -57879,7 +57879,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="445" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
         <v>333</v>
       </c>
@@ -57986,7 +57986,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="446" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
         <v>333</v>
       </c>
@@ -58093,7 +58093,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="447" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
         <v>333</v>
       </c>
@@ -58200,7 +58200,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="448" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
         <v>333</v>
       </c>
@@ -58307,7 +58307,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="449" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
         <v>333</v>
       </c>
@@ -58414,7 +58414,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="450" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
         <v>333</v>
       </c>
@@ -58521,7 +58521,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="451" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
         <v>333</v>
       </c>
@@ -58628,7 +58628,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="452" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
         <v>333</v>
       </c>
@@ -58735,7 +58735,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="453" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
         <v>333</v>
       </c>
@@ -58842,7 +58842,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="454" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
         <v>333</v>
       </c>
@@ -58949,7 +58949,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="455" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
         <v>333</v>
       </c>
@@ -59056,7 +59056,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="456" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
         <v>333</v>
       </c>
@@ -59163,7 +59163,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="457" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
         <v>333</v>
       </c>
@@ -59270,7 +59270,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="458" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
         <v>333</v>
       </c>
@@ -59377,7 +59377,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="459" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
         <v>333</v>
       </c>
@@ -59484,7 +59484,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="460" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
         <v>333</v>
       </c>
@@ -59591,7 +59591,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="461" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
         <v>333</v>
       </c>
@@ -59698,7 +59698,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="462" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
         <v>333</v>
       </c>
@@ -59805,7 +59805,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="463" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
         <v>333</v>
       </c>
@@ -59912,7 +59912,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="464" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
         <v>333</v>
       </c>
@@ -60019,7 +60019,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="465" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
         <v>333</v>
       </c>
@@ -60126,7 +60126,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="466" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
         <v>333</v>
       </c>
@@ -60233,7 +60233,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="467" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
         <v>333</v>
       </c>
@@ -60340,7 +60340,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="468" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
         <v>333</v>
       </c>
@@ -60447,7 +60447,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="469" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
         <v>333</v>
       </c>
@@ -60554,7 +60554,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="470" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
         <v>333</v>
       </c>
@@ -60661,7 +60661,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="471" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
         <v>319</v>
       </c>
@@ -60768,7 +60768,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="472" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
         <v>319</v>
       </c>
@@ -60875,7 +60875,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="473" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
         <v>319</v>
       </c>
@@ -60982,7 +60982,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="474" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
         <v>319</v>
       </c>
@@ -61089,7 +61089,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="475" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
         <v>319</v>
       </c>
@@ -61196,7 +61196,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="476" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
         <v>319</v>
       </c>
@@ -61303,7 +61303,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="477" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
         <v>319</v>
       </c>
@@ -61410,7 +61410,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="478" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
         <v>319</v>
       </c>
@@ -61517,7 +61517,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="479" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
         <v>319</v>
       </c>
@@ -61624,7 +61624,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="480" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
         <v>319</v>
       </c>
@@ -61731,7 +61731,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="481" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
         <v>319</v>
       </c>
@@ -61838,7 +61838,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="482" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
         <v>319</v>
       </c>
@@ -61945,7 +61945,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="483" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
         <v>319</v>
       </c>
@@ -62052,7 +62052,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="484" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
         <v>319</v>
       </c>
@@ -62159,7 +62159,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="485" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
         <v>319</v>
       </c>
@@ -62266,7 +62266,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="486" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
         <v>319</v>
       </c>
@@ -62373,7 +62373,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="487" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
         <v>295</v>
       </c>
@@ -62480,7 +62480,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="488" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
         <v>295</v>
       </c>
@@ -62587,7 +62587,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="489" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
         <v>282</v>
       </c>
@@ -62694,7 +62694,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="490" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
         <v>282</v>
       </c>
@@ -62801,7 +62801,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="491" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
         <v>282</v>
       </c>
@@ -62908,7 +62908,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="492" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
         <v>282</v>
       </c>
@@ -63015,7 +63015,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="493" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
         <v>282</v>
       </c>
@@ -63122,7 +63122,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="494" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
         <v>282</v>
       </c>
@@ -63229,7 +63229,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="495" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
         <v>282</v>
       </c>
@@ -63336,7 +63336,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="496" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
         <v>282</v>
       </c>
@@ -63443,7 +63443,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="497" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
         <v>282</v>
       </c>
@@ -63550,7 +63550,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="498" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
         <v>282</v>
       </c>
@@ -63657,7 +63657,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="499" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A499" t="s">
         <v>282</v>
       </c>
@@ -63764,7 +63764,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="500" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
         <v>282</v>
       </c>
@@ -63871,7 +63871,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="501" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
         <v>282</v>
       </c>
@@ -63978,7 +63978,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="502" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
         <v>282</v>
       </c>
@@ -64085,7 +64085,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="503" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
         <v>282</v>
       </c>
@@ -64192,7 +64192,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="504" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
         <v>282</v>
       </c>
@@ -64299,7 +64299,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="505" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
         <v>282</v>
       </c>
@@ -64406,7 +64406,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="506" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
         <v>282</v>
       </c>
@@ -64513,7 +64513,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="507" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
         <v>282</v>
       </c>
@@ -64620,7 +64620,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="508" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
         <v>282</v>
       </c>
@@ -64727,7 +64727,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="509" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
         <v>282</v>
       </c>
@@ -64834,7 +64834,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="510" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
         <v>282</v>
       </c>
@@ -64941,7 +64941,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="511" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
         <v>282</v>
       </c>
@@ -65048,7 +65048,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="512" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
         <v>282</v>
       </c>
@@ -65155,7 +65155,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="513" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
         <v>282</v>
       </c>
@@ -65262,7 +65262,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="514" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
         <v>282</v>
       </c>
@@ -65369,7 +65369,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="515" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A515" t="s">
         <v>282</v>
       </c>
@@ -65476,7 +65476,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="516" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A516" t="s">
         <v>282</v>
       </c>
@@ -65583,7 +65583,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="517" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A517" t="s">
         <v>282</v>
       </c>
@@ -65690,7 +65690,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="518" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A518" t="s">
         <v>282</v>
       </c>
@@ -65797,7 +65797,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="519" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A519" t="s">
         <v>282</v>
       </c>
@@ -65904,7 +65904,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="520" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A520" t="s">
         <v>282</v>
       </c>
@@ -66011,7 +66011,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="521" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A521" t="s">
         <v>282</v>
       </c>
@@ -66118,7 +66118,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="522" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A522" t="s">
         <v>282</v>
       </c>
@@ -66225,7 +66225,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="523" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A523" t="s">
         <v>282</v>
       </c>
@@ -66332,7 +66332,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="524" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A524" t="s">
         <v>282</v>
       </c>
@@ -66439,7 +66439,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="525" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="525" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A525" t="s">
         <v>282</v>
       </c>
@@ -66546,7 +66546,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="526" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="526" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A526" t="s">
         <v>282</v>
       </c>
@@ -66653,7 +66653,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="527" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="527" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A527" t="s">
         <v>282</v>
       </c>
@@ -66760,7 +66760,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="528" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="528" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A528" t="s">
         <v>282</v>
       </c>
@@ -66867,7 +66867,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="529" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="529" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A529" t="s">
         <v>282</v>
       </c>
@@ -66974,7 +66974,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="530" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A530" t="s">
         <v>282</v>
       </c>
@@ -67081,7 +67081,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="531" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="531" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A531" t="s">
         <v>282</v>
       </c>
@@ -67188,7 +67188,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="532" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="532" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A532" t="s">
         <v>282</v>
       </c>
@@ -67295,7 +67295,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="533" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="533" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A533" t="s">
         <v>282</v>
       </c>
@@ -67402,7 +67402,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="534" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="534" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
         <v>282</v>
       </c>
@@ -67509,7 +67509,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="535" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="535" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A535" t="s">
         <v>282</v>
       </c>
@@ -67616,7 +67616,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="536" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="536" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A536" t="s">
         <v>282</v>
       </c>
@@ -67723,7 +67723,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="537" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="537" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
         <v>282</v>
       </c>
@@ -67830,7 +67830,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="538" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="538" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A538" t="s">
         <v>282</v>
       </c>
@@ -67937,7 +67937,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="539" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="539" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A539" t="s">
         <v>282</v>
       </c>
@@ -68044,7 +68044,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="540" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="540" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A540" t="s">
         <v>282</v>
       </c>
@@ -68151,7 +68151,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="541" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="541" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A541" t="s">
         <v>282</v>
       </c>
@@ -68258,7 +68258,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="542" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="542" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A542" t="s">
         <v>282</v>
       </c>
@@ -68472,7 +68472,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="544" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="544" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A544" t="s">
         <v>282</v>
       </c>
@@ -68579,7 +68579,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="545" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="545" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A545" t="s">
         <v>282</v>
       </c>
@@ -68686,7 +68686,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="546" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="546" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A546" t="s">
         <v>282</v>
       </c>
@@ -68793,7 +68793,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="547" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="547" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A547" t="s">
         <v>282</v>
       </c>
@@ -68900,7 +68900,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="548" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="548" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A548" t="s">
         <v>282</v>
       </c>
@@ -69114,7 +69114,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="550" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="550" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A550" t="s">
         <v>282</v>
       </c>
@@ -69221,7 +69221,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="551" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="551" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A551" t="s">
         <v>282</v>
       </c>
@@ -69328,7 +69328,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="552" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="552" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A552" t="s">
         <v>282</v>
       </c>
@@ -69435,7 +69435,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="553" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="553" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A553" t="s">
         <v>282</v>
       </c>
@@ -69542,7 +69542,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="554" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="554" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A554" t="s">
         <v>282</v>
       </c>
@@ -69649,7 +69649,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="555" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="555" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A555" t="s">
         <v>372</v>
       </c>
@@ -69756,7 +69756,7 @@
         <v>2557</v>
       </c>
     </row>
-    <row r="556" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="556" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A556" t="s">
         <v>372</v>
       </c>
@@ -69970,7 +69970,7 @@
         <v>2557</v>
       </c>
     </row>
-    <row r="558" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="558" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A558" t="s">
         <v>372</v>
       </c>
@@ -70077,7 +70077,7 @@
         <v>2557</v>
       </c>
     </row>
-    <row r="559" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="559" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A559" t="s">
         <v>372</v>
       </c>
@@ -70291,7 +70291,7 @@
         <v>2557</v>
       </c>
     </row>
-    <row r="561" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="561" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A561" t="s">
         <v>295</v>
       </c>
@@ -70398,7 +70398,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="562" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="562" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A562" t="s">
         <v>295</v>
       </c>
@@ -70505,7 +70505,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="563" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="563" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A563" t="s">
         <v>295</v>
       </c>
@@ -70612,7 +70612,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="564" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="564" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A564" t="s">
         <v>295</v>
       </c>
@@ -70719,7 +70719,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="565" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="565" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A565" t="s">
         <v>295</v>
       </c>
@@ -70826,7 +70826,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="566" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="566" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A566" t="s">
         <v>295</v>
       </c>
@@ -70933,7 +70933,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="567" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="567" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A567" t="s">
         <v>295</v>
       </c>
@@ -71040,7 +71040,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="568" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="568" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A568" t="s">
         <v>295</v>
       </c>
@@ -71147,7 +71147,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="569" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="569" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A569" t="s">
         <v>295</v>
       </c>
@@ -71254,7 +71254,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="570" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="570" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A570" t="s">
         <v>295</v>
       </c>
@@ -71361,7 +71361,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="571" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="571" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A571" t="s">
         <v>295</v>
       </c>
@@ -71468,7 +71468,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="572" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="572" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A572" t="s">
         <v>295</v>
       </c>
@@ -71575,7 +71575,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="573" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="573" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A573" t="s">
         <v>295</v>
       </c>
@@ -76604,7 +76604,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="620" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="620" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A620" t="s">
         <v>348</v>
       </c>
@@ -76711,7 +76711,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="621" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="621" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A621" t="s">
         <v>348</v>
       </c>
@@ -80028,7 +80028,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="652" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="652" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A652" t="s">
         <v>351</v>
       </c>
@@ -80135,7 +80135,7 @@
         <v>2252</v>
       </c>
     </row>
-    <row r="653" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="653" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A653" t="s">
         <v>351</v>
       </c>
@@ -80242,7 +80242,7 @@
         <v>2253</v>
       </c>
     </row>
-    <row r="654" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="654" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A654" t="s">
         <v>351</v>
       </c>
@@ -80349,7 +80349,7 @@
         <v>2254</v>
       </c>
     </row>
-    <row r="655" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="655" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A655" t="s">
         <v>351</v>
       </c>
@@ -80456,7 +80456,7 @@
         <v>2252</v>
       </c>
     </row>
-    <row r="656" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="656" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A656" t="s">
         <v>351</v>
       </c>
@@ -80563,7 +80563,7 @@
         <v>2253</v>
       </c>
     </row>
-    <row r="657" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="657" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A657" t="s">
         <v>351</v>
       </c>
@@ -80670,7 +80670,7 @@
         <v>2254</v>
       </c>
     </row>
-    <row r="658" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="658" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A658" t="s">
         <v>351</v>
       </c>
@@ -80777,7 +80777,7 @@
         <v>2252</v>
       </c>
     </row>
-    <row r="659" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="659" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A659" t="s">
         <v>351</v>
       </c>
@@ -80884,7 +80884,7 @@
         <v>2253</v>
       </c>
     </row>
-    <row r="660" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="660" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A660" t="s">
         <v>351</v>
       </c>
@@ -80991,7 +80991,7 @@
         <v>2254</v>
       </c>
     </row>
-    <row r="661" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="661" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A661" t="s">
         <v>354</v>
       </c>
@@ -81098,7 +81098,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="662" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="662" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A662" t="s">
         <v>354</v>
       </c>
@@ -81205,7 +81205,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="663" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="663" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A663" t="s">
         <v>354</v>
       </c>
@@ -81312,7 +81312,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="664" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="664" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A664" t="s">
         <v>354</v>
       </c>
@@ -87515,7 +87515,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="722" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="722" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A722" t="s">
         <v>120</v>
       </c>
@@ -87622,7 +87622,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="723" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="723" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A723" t="s">
         <v>120</v>
       </c>
@@ -87729,7 +87729,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="724" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="724" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A724" t="s">
         <v>120</v>
       </c>
@@ -87836,7 +87836,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="725" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="725" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A725" t="s">
         <v>120</v>
       </c>
@@ -87943,7 +87943,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="726" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="726" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A726" t="s">
         <v>120</v>
       </c>
@@ -88157,7 +88157,7 @@
         <v>5370</v>
       </c>
     </row>
-    <row r="728" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="728" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A728" t="s">
         <v>120</v>
       </c>
@@ -88264,7 +88264,7 @@
         <v>5370</v>
       </c>
     </row>
-    <row r="729" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="729" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A729" t="s">
         <v>120</v>
       </c>
@@ -88371,7 +88371,7 @@
         <v>5370</v>
       </c>
     </row>
-    <row r="730" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="730" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A730" t="s">
         <v>120</v>
       </c>
@@ -88478,7 +88478,7 @@
         <v>5370</v>
       </c>
     </row>
-    <row r="731" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="731" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A731" t="s">
         <v>120</v>
       </c>
@@ -88585,7 +88585,7 @@
         <v>5370</v>
       </c>
     </row>
-    <row r="732" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="732" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
       <c r="A732" t="s">
         <v>120</v>
       </c>
@@ -90839,6 +90839,11 @@
         <filter val="abundance"/>
         <filter val="shannon wiener"/>
         <filter val="taxonomic richness"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="5">
+      <filters blank="1">
+        <filter val="TRUE"/>
       </filters>
     </filterColumn>
     <filterColumn colId="15">

</xml_diff>